<commit_message>
css work and bug fixes
</commit_message>
<xml_diff>
--- a/assets/timeSheet-Stanley-Kenneth.xlsx
+++ b/assets/timeSheet-Stanley-Kenneth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\visualpartsdb.com\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DB1785-DCCF-4CE3-9B04-7EA7431C0EE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467655BD-86EA-46C8-B691-F45B80AD1358}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15840" tabRatio="560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="24930" windowHeight="15090" tabRatio="560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="33">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t xml:space="preserve">Worked on CSS styling issues. </t>
+  </si>
+  <si>
+    <t>Worked on registering new users. We do not allow just anyone to register so I had to create a method for an admin to send a registration request to someone. They are sent a link with a code. Once they click the link and set their password their account is created.  CSS tweaks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continued to work on the registering method. Considering restructing the method to have less database calls. </t>
   </si>
 </sst>
 </file>
@@ -829,7 +835,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +900,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -959,7 +965,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1024,7 +1030,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1089,7 +1095,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1160,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1225,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1629,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1780,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1807,11 +1813,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
+    <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>42038</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>42040</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
@@ -1819,7 +1859,7 @@
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1828,7 +1868,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E15</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +1933,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1958,7 +1998,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +2063,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2088,7 +2128,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>